<commit_message>
Commit by Cam on April 16, 2020 15:05:01
</commit_message>
<xml_diff>
--- a/Voltage vs. A.xlsx
+++ b/Voltage vs. A.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>Table 1</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>Voltage</t>
+  </si>
+  <si>
+    <t>Avg</t>
   </si>
 </sst>
 </file>
@@ -640,13 +643,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>310515</xdr:colOff>
+      <xdr:colOff>310514</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>44492</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1129665</xdr:colOff>
+      <xdr:colOff>1129664</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>34078</xdr:rowOff>
     </xdr:to>
@@ -657,7 +660,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1555114" y="7013617"/>
-        <a:ext cx="5797552" cy="4033267"/>
+        <a:ext cx="5797551" cy="4033267"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1755,7 +1758,9 @@
         <v>2</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="E2" t="s" s="4">
+        <v>3</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
@@ -1768,7 +1773,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="7">
+        <f>AVERAGE(B3:B5)</f>
+        <v>0.0603386666666667</v>
+      </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>

</xml_diff>

<commit_message>
Commit by Cam on April 16, 2020 15:15:22
</commit_message>
<xml_diff>
--- a/Voltage vs. A.xlsx
+++ b/Voltage vs. A.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Table 1</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>Std Dev</t>
   </si>
 </sst>
 </file>
@@ -1761,7 +1764,9 @@
       <c r="E2" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" t="s" s="4">
+        <v>4</v>
+      </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
@@ -1777,7 +1782,10 @@
         <f>AVERAGE(B3:B5)</f>
         <v>0.0603386666666667</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="7">
+        <f>STDEV(B3:B5)</f>
+        <v>0.008943174902311449</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">

</xml_diff>